<commit_message>
Add small neg marginal cost on storage
</commit_message>
<xml_diff>
--- a/input_files/CSP_storage_case.xlsx
+++ b/input_files/CSP_storage_case.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/var/folders/m_/v6c97p3x1mg6bmvchddj43dc0000gn/T/fz3temp-2/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/awongel/Downloads/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{93A1040D-2AE6-F744-917D-AB69246BB6B0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{03136054-AC3D-754B-AA69-D728F295CC74}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="760" windowWidth="28800" windowHeight="15760" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1209,8 +1209,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:O62"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A30" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="B53" sqref="B53"/>
+    <sheetView tabSelected="1" topLeftCell="A35" zoomScaleNormal="110" workbookViewId="0">
+      <selection activeCell="K53" sqref="K53"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>

</xml_diff>